<commit_message>
added more basic gates for load instructions
</commit_message>
<xml_diff>
--- a/Part1/ControlLogic/Proj1_control_signals(1)WORKING.xlsx
+++ b/Part1/ControlLogic/Proj1_control_signals(1)WORKING.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="108">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -119,6 +119,9 @@
     <t xml:space="preserve">s_vshift</t>
   </si>
   <si>
+    <t xml:space="preserve">s_load</t>
+  </si>
+  <si>
     <t xml:space="preserve">addi</t>
   </si>
   <si>
@@ -246,6 +249,9 @@
     <t xml:space="preserve">,0000</t>
   </si>
   <si>
+    <t xml:space="preserve">,000</t>
+  </si>
+  <si>
     <t xml:space="preserve">add</t>
   </si>
   <si>
@@ -417,6 +423,9 @@
     <t xml:space="preserve">j</t>
   </si>
   <si>
+    <t xml:space="preserve">,XXXX</t>
+  </si>
+  <si>
     <t xml:space="preserve">jal</t>
   </si>
   <si>
@@ -435,19 +444,31 @@
     <t xml:space="preserve">“100000”</t>
   </si>
   <si>
+    <t xml:space="preserve">,001</t>
+  </si>
+  <si>
     <t xml:space="preserve">lh</t>
   </si>
   <si>
     <t xml:space="preserve">“100001”</t>
   </si>
   <si>
+    <t xml:space="preserve">,011</t>
+  </si>
+  <si>
     <t xml:space="preserve">lbu</t>
   </si>
   <si>
     <t xml:space="preserve">“100100”</t>
   </si>
   <si>
+    <t xml:space="preserve">,010</t>
+  </si>
+  <si>
     <t xml:space="preserve">lhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,100</t>
   </si>
   <si>
     <t xml:space="preserve">sllv</t>
@@ -580,14 +601,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+      <selection pane="bottomRight" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,34 +701,37 @@
       <c r="R2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>0</v>
@@ -725,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>1</v>
@@ -735,76 +759,82 @@
       </c>
       <c r="R3" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="P4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0</v>
@@ -837,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" s="1" t="n">
         <v>0</v>
@@ -847,17 +877,20 @@
       </c>
       <c r="R5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -893,33 +926,36 @@
         <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R6" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0</v>
@@ -949,64 +985,67 @@
         <v>0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R7" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P8" s="1" t="n">
         <v>0</v>
       </c>
@@ -1015,23 +1054,26 @@
       </c>
       <c r="R8" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>0</v>
@@ -1061,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>0</v>
@@ -1071,17 +1113,20 @@
       </c>
       <c r="R9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -1117,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P10" s="1" t="n">
         <v>0</v>
@@ -1127,23 +1172,26 @@
       </c>
       <c r="R10" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>0</v>
@@ -1173,33 +1221,36 @@
         <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R11" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>0</v>
@@ -1229,64 +1280,67 @@
         <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R12" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="P13" s="1" t="n">
         <v>0</v>
       </c>
@@ -1295,23 +1349,26 @@
       </c>
       <c r="R13" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>0</v>
@@ -1341,64 +1398,67 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R14" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="P15" s="1" t="n">
         <v>0</v>
       </c>
@@ -1407,17 +1467,20 @@
       </c>
       <c r="R15" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -1453,64 +1516,67 @@
         <v>0</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="P16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R16" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="P17" s="1" t="n">
         <v>0</v>
       </c>
@@ -1519,23 +1585,26 @@
       </c>
       <c r="R17" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>0</v>
@@ -1565,33 +1634,36 @@
         <v>0</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R18" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>0</v>
@@ -1621,33 +1693,36 @@
         <v>0</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R19" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>0</v>
@@ -1677,27 +1752,30 @@
         <v>0</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R20" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
@@ -1715,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J21" s="1" t="n">
         <v>0</v>
@@ -1733,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P21" s="1" t="n">
         <v>0</v>
@@ -1743,17 +1821,20 @@
       </c>
       <c r="R21" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0</v>
@@ -1789,27 +1870,30 @@
         <v>0</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R22" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0</v>
@@ -1845,27 +1929,30 @@
         <v>0</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R23" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>0</v>
@@ -1883,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J24" s="1" t="n">
         <v>1</v>
@@ -1901,27 +1988,30 @@
         <v>0</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R24" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>0</v>
@@ -1939,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J25" s="1" t="n">
         <v>0</v>
@@ -1957,33 +2047,36 @@
         <v>0</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R25" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>0</v>
@@ -1995,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J26" s="1" t="n">
         <v>0</v>
@@ -2013,33 +2106,36 @@
         <v>0</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="P26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R26" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>0</v>
@@ -2051,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J27" s="1" t="n">
         <v>0</v>
@@ -2069,83 +2165,89 @@
         <v>0</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="P27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R27" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="P28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R28" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>1</v>
@@ -2181,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P29" s="1" t="n">
         <v>0</v>
@@ -2191,17 +2293,20 @@
       </c>
       <c r="R29" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>1</v>
@@ -2237,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P30" s="1" t="n">
         <v>0</v>
@@ -2247,17 +2352,20 @@
       </c>
       <c r="R30" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>1</v>
@@ -2293,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P31" s="1" t="n">
         <v>0</v>
@@ -2303,17 +2411,20 @@
       </c>
       <c r="R31" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>1</v>
@@ -2349,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P32" s="1" t="n">
         <v>0</v>
@@ -2359,23 +2470,26 @@
       </c>
       <c r="R32" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>0</v>
@@ -2405,33 +2519,36 @@
         <v>0</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P33" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R33" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>0</v>
@@ -2461,33 +2578,36 @@
         <v>0</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R34" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>0</v>
@@ -2517,16 +2637,19 @@
         <v>0</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R35" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>